<commit_message>
Updated via Automatic Word Drop
</commit_message>
<xml_diff>
--- a/content/data.xlsx
+++ b/content/data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F405"/>
+  <dimension ref="A1:F406"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12563,6 +12563,36 @@
         </is>
       </c>
     </row>
+    <row r="406">
+      <c r="A406" t="n">
+        <v>2</v>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>Abdicate</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>/ˈæb.dɪ.keɪt/</t>
+        </is>
+      </c>
+      <c r="D406" t="inlineStr">
+        <is>
+          <t>To give up a position of power</t>
+        </is>
+      </c>
+      <c r="E406" t="inlineStr">
+        <is>
+          <t>The king decided to abdicate the throne.</t>
+        </is>
+      </c>
+      <c r="F406" t="inlineStr">
+        <is>
+          <t>She abdicated her responsibilities as a leader.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>